<commit_message>
Meter Point Page Script
Meter Point Script Developed
</commit_message>
<xml_diff>
--- a/xls/DomTransactional.xlsx
+++ b/xls/DomTransactional.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14790" windowHeight="6330" tabRatio="712"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14790" windowHeight="6330" tabRatio="712" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,11 @@
     <sheet name="JobAppointment" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:N19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="57">
   <si>
     <t>Runmode</t>
   </si>
@@ -114,12 +113,6 @@
     <t>ExistingMSN</t>
   </si>
   <si>
-    <t>Installed MPRN</t>
-  </si>
-  <si>
-    <t>Removed MPRN</t>
-  </si>
-  <si>
     <t>Remove</t>
   </si>
   <si>
@@ -129,15 +122,6 @@
     <t>8347853475</t>
   </si>
   <si>
-    <t>fgdfg</t>
-  </si>
-  <si>
-    <t>dfgdfg</t>
-  </si>
-  <si>
-    <t>8247867578</t>
-  </si>
-  <si>
     <t>Cannot create Job</t>
   </si>
   <si>
@@ -147,9 +131,6 @@
     <t>IE</t>
   </si>
   <si>
-    <t>8144467559</t>
-  </si>
-  <si>
     <t>Job Appointed Successfully</t>
   </si>
   <si>
@@ -181,6 +162,36 @@
   </si>
   <si>
     <t>ie</t>
+  </si>
+  <si>
+    <t>5656555454</t>
+  </si>
+  <si>
+    <t>* A Meter is already installed on this meter point.</t>
+  </si>
+  <si>
+    <t>* Cannot exchange meter as there is no existing meter on this meter point.</t>
+  </si>
+  <si>
+    <t>1000000014</t>
+  </si>
+  <si>
+    <t>* Cannot remove meter as the meter does not exist on this meter point.</t>
+  </si>
+  <si>
+    <t>Relocation can be done only with UKMA meters. Please change work type to Relocation &amp; Exchange!</t>
+  </si>
+  <si>
+    <t>Relocation</t>
+  </si>
+  <si>
+    <t>* Cannot relocate &amp; exchange meter as there is no existing meter on this meter point.</t>
+  </si>
+  <si>
+    <t>1011100014</t>
+  </si>
+  <si>
+    <t>Relocation_And_Exchange</t>
   </si>
 </sst>
 </file>
@@ -532,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -551,7 +562,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -559,7 +570,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -591,7 +602,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -599,7 +610,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -653,7 +664,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -662,10 +673,10 @@
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -673,7 +684,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -682,10 +693,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>33</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -693,19 +704,19 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
         <v>33</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -713,19 +724,19 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -735,10 +746,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -746,10 +757,10 @@
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="92" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -789,18 +800,16 @@
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
+        <v>47</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -812,18 +821,15 @@
         <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
+        <v>50</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -832,21 +838,18 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
@@ -855,21 +858,18 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
+        <v>50</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
@@ -878,16 +878,33 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -938,13 +955,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -993,13 +1010,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1164,16 +1181,16 @@
         <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>